<commit_message>
new paper, viz and cv
</commit_message>
<xml_diff>
--- a/resources.xlsx
+++ b/resources.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucfnmac_ucl_ac_uk/Documents/General/website/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy\OneDrive - University College London\General\website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="14_{753DDDC7-04B4-43F4-8EA7-A447851C672E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F8FD299-6695-4FE0-8608-27A2ECB36029}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C47ABF-ACC7-4105-A9A2-693E46DC2D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14025" yWindow="4230" windowWidth="43200" windowHeight="12330" xr2:uid="{6362DE6B-9A95-49B5-8331-B8A2B0F11EDC}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="17460" windowHeight="10260" xr2:uid="{6362DE6B-9A95-49B5-8331-B8A2B0F11EDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -272,9 +272,6 @@
     <t>Figure code</t>
   </si>
   <si>
-    <t>Study area</t>
-  </si>
-  <si>
     <t>Icon</t>
   </si>
   <si>
@@ -300,6 +297,9 @@
   </si>
   <si>
     <t>Spatial analysis of public health data book</t>
+  </si>
+  <si>
+    <t>Figure 1. True colour composite airborne hyperspectral mosaics collected during the Wytham Woods 2021 (top left), Wytham Woods 2018 (middle left), and Valencia Anchor Station 2017 (bottom left) campaigns, in addition to the location of the elementary sampling units (ESUs) in which in situ LAI and LCC measurements were performed (middle), and the location of each study site (right)</t>
   </si>
 </sst>
 </file>
@@ -375,10 +375,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -700,19 +696,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B245866-484B-4C42-BB5F-73A7295E0F38}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="E16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="14.26953125" customWidth="1"/>
+    <col min="7" max="7" width="37.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -729,7 +725,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>8</v>
@@ -738,7 +734,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -752,7 +748,7 @@
         <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G2" t="s">
         <v>42</v>
@@ -761,7 +757,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -775,7 +771,7 @@
         <v>57</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
         <v>56</v>
@@ -784,7 +780,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -798,7 +794,7 @@
         <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s">
         <v>15</v>
@@ -807,7 +803,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -824,7 +820,7 @@
         <v>72</v>
       </c>
       <c r="F5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s">
         <v>61</v>
@@ -833,7 +829,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -850,7 +846,7 @@
         <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G6" t="s">
         <v>59</v>
@@ -859,7 +855,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -876,16 +872,16 @@
         <v>73</v>
       </c>
       <c r="F7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -902,7 +898,7 @@
         <v>73</v>
       </c>
       <c r="F8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G8" t="s">
         <v>17</v>
@@ -911,7 +907,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -928,16 +924,16 @@
         <v>74</v>
       </c>
       <c r="F9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -954,7 +950,7 @@
         <v>74</v>
       </c>
       <c r="F10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G10" t="s">
         <v>22</v>
@@ -963,7 +959,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -980,7 +976,7 @@
         <v>74</v>
       </c>
       <c r="F11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G11" t="s">
         <v>24</v>
@@ -989,7 +985,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1006,7 +1002,7 @@
         <v>74</v>
       </c>
       <c r="F12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G12" t="s">
         <v>25</v>
@@ -1015,7 +1011,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1032,7 +1028,7 @@
         <v>74</v>
       </c>
       <c r="F13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G13" t="s">
         <v>26</v>
@@ -1041,7 +1037,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1058,7 +1054,7 @@
         <v>74</v>
       </c>
       <c r="F14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G14" t="s">
         <v>27</v>
@@ -1067,7 +1063,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1084,7 +1080,7 @@
         <v>74</v>
       </c>
       <c r="F15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G15" t="s">
         <v>28</v>
@@ -1093,7 +1089,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1110,7 +1106,7 @@
         <v>74</v>
       </c>
       <c r="F16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G16" t="s">
         <v>29</v>
@@ -1119,7 +1115,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1136,7 +1132,7 @@
         <v>74</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G17" t="s">
         <v>30</v>
@@ -1145,7 +1141,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1162,7 +1158,7 @@
         <v>74</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G18" t="s">
         <v>31</v>
@@ -1171,7 +1167,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1188,16 +1184,16 @@
         <v>75</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1214,7 +1210,7 @@
         <v>75</v>
       </c>
       <c r="F20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G20" t="s">
         <v>47</v>
@@ -1223,7 +1219,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
@@ -1237,16 +1233,16 @@
         <v>73</v>
       </c>
       <c r="F21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A22" s="1" t="s">
         <v>45</v>
       </c>
@@ -1260,7 +1256,7 @@
         <v>73</v>
       </c>
       <c r="F22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G22" t="s">
         <v>51</v>
@@ -1269,7 +1265,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -1283,7 +1279,7 @@
         <v>76</v>
       </c>
       <c r="F23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G23" t="s">
         <v>65</v>
@@ -1292,7 +1288,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -1306,16 +1302,16 @@
         <v>77</v>
       </c>
       <c r="F24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G24" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="H24" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -1332,7 +1328,7 @@
         <v>77</v>
       </c>
       <c r="F25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G25" t="s">
         <v>70</v>

</xml_diff>